<commit_message>
workflow diary, deleted copies
</commit_message>
<xml_diff>
--- a/pracovný denník.xlsx
+++ b/pracovný denník.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAX\Desktop\School\_Diplomová práca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAX\Desktop\SCHOOL\_Diplomová práca\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>Dátum</t>
   </si>
@@ -38,26 +38,140 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Literatúra [1] - časť Automatic Speech Recognition a Natural language processing (poznámky a časti do citácie)</t>
-  </si>
-  <si>
     <t>Literatúra [2] - Speech recognition (poznámky a časti do citácie)</t>
   </si>
   <si>
     <t>In progress</t>
   </si>
   <si>
-    <t>Literatúra [3] - technológie prevodu</t>
+    <t>15.1.2025</t>
+  </si>
+  <si>
+    <t>2.2.2025</t>
+  </si>
+  <si>
+    <t>Literatúra [1] - Automatic Speech Recognition a Natural language processing (poznámky a časti do citácie)</t>
+  </si>
+  <si>
+    <t>Literatúra [3] - ASR postupy (poznámky a časti do citácie)</t>
+  </si>
+  <si>
+    <t>Literatúra [4] - Technológie modelov STT (poznámky a časti do citácie)</t>
+  </si>
+  <si>
+    <t>Literatúra [5] (poznámky a časti do citácie)</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>Inštalácia Whisper OpenAI</t>
+  </si>
+  <si>
+    <t>Inštalácia Python SpeechRecognition</t>
+  </si>
+  <si>
+    <t>Inštalácia Wav2vec</t>
+  </si>
+  <si>
+    <t>Python module pre Whisper</t>
+  </si>
+  <si>
+    <t>Inštalácia Kaldi</t>
+  </si>
+  <si>
+    <t>Rework</t>
+  </si>
+  <si>
+    <t>5.1.2025</t>
+  </si>
+  <si>
+    <t>26.2.2025</t>
+  </si>
+  <si>
+    <t>28.2.2025</t>
+  </si>
+  <si>
+    <t>Main Python testing script + JSON output</t>
+  </si>
+  <si>
+    <t>1.3.2025</t>
+  </si>
+  <si>
+    <t>Python module pre Kaldi (WSL)</t>
+  </si>
+  <si>
+    <t>Výber testovacieho materiálu (Common voice)</t>
+  </si>
+  <si>
+    <t>Filtrovanie validated materiálu</t>
+  </si>
+  <si>
+    <t>Python script na vytváranie kontrolného JSON file</t>
+  </si>
+  <si>
+    <t>Rozdelenie diplomovej práce na teoretickú a praktickú časť, predpripraviť kapitoly a podkapitoly</t>
+  </si>
+  <si>
+    <t>Testovacia fáza, opakovanie testov</t>
+  </si>
+  <si>
+    <t>Diplomová práca do aktuálnej šablóny</t>
+  </si>
+  <si>
+    <t>Rozdelenie citácií do podkapitol teoretickej časti DP</t>
+  </si>
+  <si>
+    <t>Koncept praktickej časti do kapitol DP</t>
+  </si>
+  <si>
+    <t>Python script na porovnávanie výsledkov s kontrolnými dátami</t>
+  </si>
+  <si>
+    <t>Duplikovanie testovacieho materiálu, modifikácia (zmena rýchlosti + a -, pridávanie šumu) - (Python script?)</t>
+  </si>
+  <si>
+    <t>Porovnávanie výsledkov s kontrolnými dátami, vyhodnotenie úspešnosti, vyhodnotenie vplyvu rušivých elementov</t>
+  </si>
+  <si>
+    <t>Výstup z dát, vizualizácia, závery z testov</t>
+  </si>
+  <si>
+    <t>Rozšíriť teoretickú časť, technológie STT, typy modelov, história vývoja, aplikácia a preklad citácií</t>
+  </si>
+  <si>
+    <t>Python module pre Wav2vec (pridať podporu ďalších modelov vo Wav2vec)</t>
+  </si>
+  <si>
+    <t>Python module pre Python SpeechRecognition (podpora 10 modelov)</t>
+  </si>
+  <si>
+    <t>Zmeny a aktuálny stav Diplomovej práce dostupný na:</t>
+  </si>
+  <si>
+    <t>https://github.com/JurajKralik/diplomova_praca</t>
+  </si>
+  <si>
+    <t>Online zdroje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -72,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -209,11 +323,126 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -221,35 +450,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -290,6 +545,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <fgColor auto="1"/>
           <bgColor theme="9"/>
         </patternFill>
@@ -298,7 +574,43 @@
     <dxf>
       <fill>
         <patternFill>
-          <fgColor theme="9"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -578,70 +890,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="6" customWidth="1"/>
     <col min="2" max="2" width="100.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>45672</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="E1" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>45678</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="C1:C16 C21:C1048576 C18">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"Rework"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"Rework"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"To do"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:C20">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Rework"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"To do"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>